<commit_message>
Fix: map Chaudière -> F28 and PDB 3 -> H28; update Excel template export
</commit_message>
<xml_diff>
--- a/public/Electrical Consumption.xlsx
+++ b/public/Electrical Consumption.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Msi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Msi\Desktop\electrical-consumption-reporter\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0C1235-AF6F-4AF3-8394-53BCA2A1F519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7EF638-F128-4A04-89D8-1AE516EFB8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{3D1C84FC-D0D6-48B3-9275-4A3111EEBB06}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Electrical Consumption Reporting</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Salle du transformateur 2</t>
+  </si>
+  <si>
+    <t>Chaudière</t>
   </si>
 </sst>
 </file>
@@ -431,23 +434,23 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -843,8 +846,8 @@
   </sheetPr>
   <dimension ref="B3:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -861,13 +864,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="4" t="s">
         <v>5</v>
       </c>
@@ -876,11 +879,11 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="5"/>
       <c r="H4" s="2"/>
     </row>
@@ -896,7 +899,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -905,42 +908,42 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="2:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="18"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="2:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="18"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="2:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="18"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="18"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="18"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="18"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="8" t="s">
         <v>10</v>
       </c>
@@ -953,8 +956,8 @@
       <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="14">
         <f>F6+F7+F8+F12</f>
         <v>0</v>
@@ -963,7 +966,7 @@
     </row>
     <row r="14" spans="2:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="11"/>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="17" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="7" t="s">
@@ -972,7 +975,7 @@
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="2:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D15" s="16"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="7" t="s">
         <v>16</v>
       </c>
@@ -982,14 +985,14 @@
       <c r="C16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="14">
         <f>F14+F15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="11"/>
       <c r="D17" s="3" t="s">
         <v>19</v>
@@ -999,19 +1002,19 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="3:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:8" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="14">
         <f>F17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="16" t="s">
+    <row r="19" spans="3:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -1019,15 +1022,15 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="16"/>
+    <row r="20" spans="3:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="17"/>
       <c r="E20" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="3:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="16"/>
+    <row r="21" spans="3:8" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="17"/>
       <c r="E21" s="5" t="s">
         <v>7</v>
       </c>
@@ -1036,8 +1039,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="16"/>
+    <row r="22" spans="3:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="17"/>
       <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
@@ -1046,18 +1049,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="14">
         <f>F19+F20+F21+F22</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:8" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
         <v>26</v>
       </c>
@@ -1066,18 +1069,18 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="3:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
       <c r="F25" s="14">
         <f>F24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
         <v>29</v>
       </c>
@@ -1086,39 +1089,43 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="3:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:8" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
       <c r="F27" s="14">
         <f>F26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D28" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E28" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="3:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="3:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="14">
         <f>F28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="16" t="s">
+    <row r="30" spans="3:8" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="7" t="s">
@@ -1126,8 +1133,8 @@
       </c>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="3:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="16"/>
+    <row r="31" spans="3:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="17"/>
       <c r="E31" s="7" t="s">
         <v>36</v>
       </c>
@@ -1136,8 +1143,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="16"/>
+    <row r="32" spans="3:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="17"/>
       <c r="E32" s="7" t="s">
         <v>37</v>
       </c>
@@ -1147,7 +1154,7 @@
       </c>
     </row>
     <row r="33" spans="3:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="16"/>
+      <c r="D33" s="17"/>
       <c r="E33" s="7" t="s">
         <v>23</v>
       </c>
@@ -1157,28 +1164,28 @@
       </c>
     </row>
     <row r="34" spans="3:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="16"/>
+      <c r="D34" s="17"/>
       <c r="E34" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="3:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="16"/>
+      <c r="D35" s="17"/>
       <c r="E35" s="7" t="s">
         <v>39</v>
       </c>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="3:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="16"/>
+      <c r="D36" s="17"/>
       <c r="E36" s="7" t="s">
         <v>41</v>
       </c>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="3:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="16"/>
+      <c r="D37" s="17"/>
       <c r="E37" s="7" t="s">
         <v>42</v>
       </c>
@@ -1191,8 +1198,8 @@
       <c r="C38" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="14">
         <f>F30+F35+F37</f>
         <v>0</v>
@@ -1211,8 +1218,8 @@
       <c r="C40" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
       <c r="F40" s="14">
         <f>F39</f>
         <v>0</v>
@@ -1238,6 +1245,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:D37"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="D6:D12"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="D3:F4"/>
@@ -1246,13 +1260,6 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:D37"/>
-    <mergeCell ref="D38:E38"/>
   </mergeCells>
   <pageMargins left="0.23622047244094488" right="0.23622047244094488" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="66" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>